<commit_message>
im back from the dead
</commit_message>
<xml_diff>
--- a/pypl.xlsx
+++ b/pypl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacharles\Desktop\work\models\financial_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36431956-E202-46F1-9D13-0BBAB785A6FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A39B1B-7F97-437F-B8AC-73837BDC251B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19410" yWindow="1215" windowWidth="18555" windowHeight="12300" activeTab="1" xr2:uid="{696C57CC-035B-4707-BC42-086A1379E7B4}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{696C57CC-035B-4707-BC42-086A1379E7B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
   <si>
     <t xml:space="preserve">Paypal </t>
   </si>
@@ -244,6 +244,30 @@
   </si>
   <si>
     <t>payouts</t>
+  </si>
+  <si>
+    <t>q123</t>
+  </si>
+  <si>
+    <t>q223</t>
+  </si>
+  <si>
+    <t>q323</t>
+  </si>
+  <si>
+    <t>q423</t>
+  </si>
+  <si>
+    <t>q124</t>
+  </si>
+  <si>
+    <t>q224</t>
+  </si>
+  <si>
+    <t>q324</t>
+  </si>
+  <si>
+    <t>q424</t>
   </si>
 </sst>
 </file>
@@ -323,6 +347,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>604157</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>97971</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9AA8C9D-7923-BD69-4CE8-14A0E17DE060}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5508171" y="38100"/>
+          <a:ext cx="5443" cy="8441871"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -642,15 +721,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{620FF8CA-6AAA-4819-A3BA-551B7F44D6E8}">
-  <dimension ref="B2:I45"/>
+  <dimension ref="B2:J45"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -658,50 +737,54 @@
         <v>27</v>
       </c>
       <c r="I2">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+        <v>86.65</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H3" t="s">
         <v>28</v>
       </c>
       <c r="I3">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H4" t="s">
         <v>29</v>
       </c>
       <c r="I4">
         <f>I3*I2</f>
-        <v>81760</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+        <v>86823.3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H5" t="s">
         <v>16</v>
       </c>
       <c r="I5">
+        <f>7272+4647</f>
+        <v>11919</v>
+      </c>
+      <c r="J5">
         <f>7701+5915</f>
         <v>13616</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H6" t="s">
         <v>30</v>
       </c>
       <c r="I6">
-        <v>50713</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+        <v>50268</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H7" t="s">
         <v>31</v>
       </c>
       <c r="I7">
         <f>I4-I5+I6</f>
-        <v>118857</v>
+        <v>125172.3</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -851,13 +934,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B59426AB-9D68-4270-9D58-A65E35156EA7}">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:Q46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="I24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G31" sqref="G31"/>
+      <selection pane="bottomRight" activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,12 +950,12 @@
     <col min="5" max="7" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
         <v>2018</v>
       </c>
@@ -897,8 +980,32 @@
         <f t="shared" si="0"/>
         <v>2024</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O2" t="s">
+        <v>74</v>
+      </c>
+      <c r="P2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -922,7 +1029,7 @@
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -946,7 +1053,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -970,7 +1077,7 @@
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -994,7 +1101,7 @@
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -1024,13 +1131,13 @@
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1056,7 +1163,7 @@
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1082,7 +1189,7 @@
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1108,13 +1215,13 @@
       </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D13">
         <v>-1</v>
       </c>
@@ -1123,7 +1230,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1145,8 +1252,26 @@
       <c r="G14" s="2">
         <v>29771</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="2">
+        <v>7040</v>
+      </c>
+      <c r="K14" s="2">
+        <v>7287</v>
+      </c>
+      <c r="L14" s="2">
+        <v>7418</v>
+      </c>
+      <c r="N14" s="2">
+        <v>7699</v>
+      </c>
+      <c r="O14" s="2">
+        <v>7885</v>
+      </c>
+      <c r="P14" s="2">
+        <v>7847</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1168,8 +1293,26 @@
       <c r="G15" s="2">
         <v>-14385</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="2">
+        <v>-3283</v>
+      </c>
+      <c r="K15" s="2">
+        <v>-3541</v>
+      </c>
+      <c r="L15" s="2">
+        <v>-3603</v>
+      </c>
+      <c r="N15" s="2">
+        <v>-3917</v>
+      </c>
+      <c r="O15" s="2">
+        <v>-3942</v>
+      </c>
+      <c r="P15" s="2">
+        <v>-3841</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1191,8 +1334,26 @@
       <c r="G16" s="2">
         <v>-1682</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J16" s="2">
+        <v>-442</v>
+      </c>
+      <c r="K16" s="2">
+        <v>-398</v>
+      </c>
+      <c r="L16" s="2">
+        <v>-446</v>
+      </c>
+      <c r="N16" s="2">
+        <v>-321</v>
+      </c>
+      <c r="O16" s="2">
+        <v>-335</v>
+      </c>
+      <c r="P16" s="2">
+        <v>-352</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1214,8 +1375,26 @@
       <c r="G17" s="2">
         <v>-1919</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J17" s="2">
+        <v>-488</v>
+      </c>
+      <c r="K17" s="2">
+        <v>-492</v>
+      </c>
+      <c r="L17" s="2">
+        <v>-474</v>
+      </c>
+      <c r="N17" s="2">
+        <v>-454</v>
+      </c>
+      <c r="O17" s="2">
+        <v>-436</v>
+      </c>
+      <c r="P17" s="2">
+        <v>-427</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1237,8 +1416,26 @@
       <c r="G18" s="2">
         <v>-1809</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J18" s="2">
+        <v>-436</v>
+      </c>
+      <c r="K18" s="2">
+        <v>-465</v>
+      </c>
+      <c r="L18" s="2">
+        <v>-442</v>
+      </c>
+      <c r="N18" s="2">
+        <v>-421</v>
+      </c>
+      <c r="O18" s="2">
+        <v>-446</v>
+      </c>
+      <c r="P18" s="2">
+        <v>-508</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1260,8 +1457,26 @@
       <c r="G19" s="2">
         <v>-2973</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J19" s="2">
+        <v>-721</v>
+      </c>
+      <c r="K19" s="2">
+        <v>-743</v>
+      </c>
+      <c r="L19" s="2">
+        <v>-739</v>
+      </c>
+      <c r="N19" s="2">
+        <v>-742</v>
+      </c>
+      <c r="O19" s="2">
+        <v>-718</v>
+      </c>
+      <c r="P19" s="2">
+        <v>-746</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1284,8 +1499,26 @@
         <v>-2059</v>
       </c>
       <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J20" s="2">
+        <v>-507</v>
+      </c>
+      <c r="K20" s="2">
+        <v>-491</v>
+      </c>
+      <c r="L20" s="2">
+        <v>-507</v>
+      </c>
+      <c r="N20" s="2">
+        <v>-464</v>
+      </c>
+      <c r="O20" s="2">
+        <v>-570</v>
+      </c>
+      <c r="P20" s="2">
+        <v>-519</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1307,8 +1540,26 @@
       <c r="G21" s="2">
         <v>84</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J21" s="2">
+        <v>-164</v>
+      </c>
+      <c r="K21" s="2">
+        <v>-24</v>
+      </c>
+      <c r="L21" s="2">
+        <v>-39</v>
+      </c>
+      <c r="N21" s="2">
+        <v>-212</v>
+      </c>
+      <c r="O21" s="2">
+        <v>-113</v>
+      </c>
+      <c r="P21" s="2">
+        <v>-63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -1336,8 +1587,32 @@
         <f t="shared" si="7"/>
         <v>5028</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J22" s="3">
+        <f t="shared" ref="J22" si="8">SUM(J14:J21)</f>
+        <v>999</v>
+      </c>
+      <c r="K22" s="3">
+        <f t="shared" ref="K22:L22" si="9">SUM(K14:K21)</f>
+        <v>1133</v>
+      </c>
+      <c r="L22" s="3">
+        <f t="shared" si="9"/>
+        <v>1168</v>
+      </c>
+      <c r="N22" s="3">
+        <f t="shared" ref="N22:O22" si="10">SUM(N14:N21)</f>
+        <v>1168</v>
+      </c>
+      <c r="O22" s="3">
+        <f t="shared" si="10"/>
+        <v>1325</v>
+      </c>
+      <c r="P22" s="3">
+        <f t="shared" ref="P22" si="11">SUM(P14:P21)</f>
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1359,8 +1634,26 @@
       <c r="G23" s="2">
         <v>383</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J23" s="2">
+        <v>41</v>
+      </c>
+      <c r="K23" s="2">
+        <v>170</v>
+      </c>
+      <c r="L23" s="2">
+        <v>73</v>
+      </c>
+      <c r="N23" s="2">
+        <v>41</v>
+      </c>
+      <c r="O23" s="2">
+        <v>74</v>
+      </c>
+      <c r="P23" s="2">
+        <v>-80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1382,21 +1675,39 @@
       <c r="G24" s="2">
         <v>-1165</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J24" s="2">
+        <v>-279</v>
+      </c>
+      <c r="K24" s="2">
+        <v>-274</v>
+      </c>
+      <c r="L24" s="2">
+        <v>-221</v>
+      </c>
+      <c r="N24" s="2">
+        <v>-321</v>
+      </c>
+      <c r="O24" s="2">
+        <v>-271</v>
+      </c>
+      <c r="P24" s="2">
+        <v>-301</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B25" s="3">
-        <f t="shared" ref="B25:D25" si="8">SUM(B22:B24)</f>
+        <f t="shared" ref="B25:D25" si="12">SUM(B22:B24)</f>
         <v>2057</v>
       </c>
       <c r="C25" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2459</v>
       </c>
       <c r="D25" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>4202</v>
       </c>
       <c r="E25" s="3">
@@ -1411,396 +1722,539 @@
         <f>SUM(G22:G24)</f>
         <v>4246</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J25" s="3">
+        <f>SUM(J22:J24)</f>
+        <v>761</v>
+      </c>
+      <c r="K25" s="3">
+        <f>SUM(K22:K24)</f>
+        <v>1029</v>
+      </c>
+      <c r="L25" s="3">
+        <f>SUM(L22:L24)</f>
+        <v>1020</v>
+      </c>
+      <c r="N25" s="3">
+        <f>SUM(N22:N24)</f>
+        <v>888</v>
+      </c>
+      <c r="O25" s="3">
+        <f>SUM(O22:O24)</f>
+        <v>1128</v>
+      </c>
+      <c r="P25" s="3">
+        <f>SUM(P22:P24)</f>
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27">
+        <v>5480</v>
+      </c>
+      <c r="C27">
+        <v>4071</v>
+      </c>
+      <c r="D27">
+        <v>5854</v>
+      </c>
+      <c r="E27" s="2">
+        <v>5797</v>
+      </c>
+      <c r="F27" s="2">
+        <v>5813</v>
+      </c>
+      <c r="G27" s="2">
+        <v>4843</v>
+      </c>
+      <c r="J27" s="2">
+        <v>1170</v>
+      </c>
+      <c r="K27">
+        <v>970</v>
+      </c>
+      <c r="L27">
+        <v>2229</v>
+      </c>
+      <c r="N27">
+        <v>1917</v>
+      </c>
+      <c r="O27">
+        <v>3442</v>
+      </c>
+      <c r="P27">
+        <v>5056</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="2">
+        <v>-823</v>
+      </c>
+      <c r="C28" s="2">
+        <v>-704</v>
+      </c>
+      <c r="D28" s="2">
+        <v>-866</v>
+      </c>
+      <c r="E28" s="2">
+        <v>-908</v>
+      </c>
+      <c r="F28" s="2">
+        <v>-706</v>
+      </c>
+      <c r="G28" s="2">
+        <v>-623</v>
+      </c>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2">
+        <v>-170</v>
+      </c>
+      <c r="K28" s="2">
+        <f>-320+40</f>
+        <v>-280</v>
+      </c>
+      <c r="L28" s="2">
+        <v>-478</v>
+      </c>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2">
+        <v>-154</v>
+      </c>
+      <c r="O28" s="2">
+        <v>-311</v>
+      </c>
+      <c r="P28" s="2">
+        <v>-480</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29">
+        <f>B27+B28</f>
+        <v>4657</v>
+      </c>
+      <c r="C29">
+        <f>C27+C28</f>
+        <v>3367</v>
+      </c>
+      <c r="D29">
+        <f>D27+D28</f>
+        <v>4988</v>
+      </c>
+      <c r="E29" s="2">
+        <f>E27+E28</f>
+        <v>4889</v>
+      </c>
+      <c r="F29" s="2">
+        <f>F27+F28</f>
+        <v>5107</v>
+      </c>
+      <c r="G29" s="2">
+        <f>G27+G28</f>
+        <v>4220</v>
+      </c>
+      <c r="J29" s="2">
+        <f>SUM(J27:J28)</f>
+        <v>1000</v>
+      </c>
+      <c r="K29">
+        <f>SUM(K27:K28)</f>
+        <v>690</v>
+      </c>
+      <c r="L29">
+        <f>SUM(L27:L28)</f>
+        <v>1751</v>
+      </c>
+      <c r="N29">
+        <f>SUM(N27:N28)</f>
+        <v>1763</v>
+      </c>
+      <c r="O29">
+        <f>SUM(O27:O28)</f>
+        <v>3131</v>
+      </c>
+      <c r="P29">
+        <f>SUM(P27:P28)</f>
+        <v>4576</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C32" s="4">
         <f>C14/B14-1</f>
         <v>0.15021681444566704</v>
       </c>
-      <c r="D27" s="4">
-        <f t="shared" ref="D27:E27" si="9">D14/C14-1</f>
+      <c r="D32" s="4">
+        <f>D14/C14-1</f>
         <v>0.20717983344586988</v>
       </c>
-      <c r="E27" s="4">
-        <f t="shared" si="9"/>
+      <c r="E32" s="4">
+        <f>E14/D14-1</f>
         <v>0.18257667567819524</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F32" s="4">
         <f>F14/E14-1</f>
         <v>8.4624177210200546E-2</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G32" s="4">
         <f>G14/F14-1</f>
         <v>8.1873682680427384E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="N32" s="4">
+        <f>N14/J14-1</f>
+        <v>9.3607954545454453E-2</v>
+      </c>
+      <c r="O32" s="4">
+        <f>O14/K14-1</f>
+        <v>8.2063949499108002E-2</v>
+      </c>
+      <c r="P32" s="4">
+        <f>P14/L14-1</f>
+        <v>5.7832299811269916E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C33" s="4">
         <f>C25/B25-1</f>
         <v>0.19543023821098693</v>
       </c>
-      <c r="D28" s="4">
-        <f t="shared" ref="D28:E28" si="10">D25/C25-1</f>
+      <c r="D33" s="4">
+        <f>D25/C25-1</f>
         <v>0.70882472549816988</v>
       </c>
-      <c r="E28" s="4">
-        <f t="shared" si="10"/>
+      <c r="E33" s="4">
+        <f>E25/D25-1</f>
         <v>-7.8534031413612926E-3</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F33" s="4">
         <f>F25/E25-1</f>
         <v>-0.41976493163828255</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G33" s="4">
         <f>G25/F25-1</f>
         <v>0.75527077304671342</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="N33" s="4">
+        <f>N25/J25-1</f>
+        <v>0.1668856767411302</v>
+      </c>
+      <c r="O33" s="4">
+        <f>O25/K25-1</f>
+        <v>9.6209912536443065E-2</v>
+      </c>
+      <c r="P33" s="4">
+        <f>P25/L25-1</f>
+        <v>-9.8039215686274161E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B34" s="4">
         <f>B22/B14</f>
         <v>0.1419972817293379</v>
       </c>
-      <c r="C29" s="4">
-        <f t="shared" ref="C29:D29" si="11">C22/C14</f>
+      <c r="C34" s="4">
+        <f>C22/C14</f>
         <v>0.15299347287868556</v>
       </c>
-      <c r="D29" s="4">
-        <f t="shared" si="11"/>
+      <c r="D34" s="4">
+        <f>D22/D14</f>
         <v>0.15330474503589075</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E34" s="4">
         <f>E22/E14</f>
         <v>0.16798707185369122</v>
       </c>
-      <c r="F29" s="4">
-        <f t="shared" ref="F29:G29" si="12">F22/F14</f>
+      <c r="F34" s="4">
+        <f>F22/F14</f>
         <v>0.13943600552365723</v>
       </c>
-      <c r="G29" s="4">
-        <f t="shared" si="12"/>
+      <c r="G34" s="4">
+        <f>G22/G14</f>
         <v>0.16888918746431092</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="J34" s="4">
+        <f>J22/J14</f>
+        <v>0.14190340909090909</v>
+      </c>
+      <c r="K34" s="4">
+        <f>K22/K14</f>
+        <v>0.15548236585700562</v>
+      </c>
+      <c r="L34" s="4">
+        <f>L22/L14</f>
+        <v>0.15745483957940146</v>
+      </c>
+      <c r="M34" s="4" t="e">
+        <f>M22/M14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N34" s="4">
+        <f>N22/N14</f>
+        <v>0.15170801402779582</v>
+      </c>
+      <c r="O34" s="4">
+        <f>O22/O14</f>
+        <v>0.16804058338617628</v>
+      </c>
+      <c r="P34" s="4">
+        <f>P22/P14</f>
+        <v>0.17726519689053141</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="4">
+        <f>C29/B29-1</f>
+        <v>-0.27700236203564521</v>
+      </c>
+      <c r="D35" s="4">
+        <f>D29/C29-1</f>
+        <v>0.48143748143748133</v>
+      </c>
+      <c r="E35" s="4">
+        <f>E29/D29-1</f>
+        <v>-1.9847634322373686E-2</v>
+      </c>
+      <c r="F35" s="4">
+        <f>F29/E29-1</f>
+        <v>4.4589895684189029E-2</v>
+      </c>
+      <c r="G35" s="4">
+        <f>G29/F29-1</f>
+        <v>-0.17368317994908944</v>
+      </c>
+      <c r="N35" s="4">
+        <f>N29/J29-1</f>
+        <v>0.7629999999999999</v>
+      </c>
+      <c r="O35" s="4">
+        <f t="shared" ref="O35:P35" si="13">O29/K29-1</f>
+        <v>3.5376811594202895</v>
+      </c>
+      <c r="P35" s="4">
+        <f t="shared" si="13"/>
+        <v>1.6133637921187893</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>16</v>
       </c>
-      <c r="C31">
+      <c r="C37">
         <f>7349+3412</f>
         <v>10761</v>
       </c>
-      <c r="D31">
+      <c r="D37">
         <f>4794+8289</f>
         <v>13083</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F37" s="2">
         <f>7776+3092</f>
         <v>10868</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G37" s="2">
         <f>9081+4979</f>
         <v>14060</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>17</v>
       </c>
-      <c r="C32">
+      <c r="C38">
         <v>435</v>
       </c>
-      <c r="D32">
+      <c r="D38">
         <v>577</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F38" s="2">
         <v>963</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G38" s="2">
         <v>1069</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="39" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>19</v>
       </c>
-      <c r="C33">
+      <c r="B39"/>
+      <c r="C39">
         <v>22527</v>
       </c>
-      <c r="D33">
+      <c r="D39">
         <v>33418</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F39" s="2">
         <v>36264</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G39" s="2">
         <v>38935</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+      <c r="N39"/>
+      <c r="O39"/>
+      <c r="P39"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>18</v>
       </c>
-      <c r="C34">
+      <c r="C40">
         <v>1693</v>
       </c>
-      <c r="D34">
+      <c r="D40">
         <v>1807</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F40" s="2">
         <v>1730</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G40" s="2">
         <v>1488</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C41" s="2">
         <v>-24527</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D41" s="2">
         <v>-35418</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F41" s="2">
         <v>-40014</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G41" s="2">
         <v>-41935</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37">
-        <f>B25</f>
-        <v>2057</v>
-      </c>
-      <c r="C37">
-        <f t="shared" ref="C37:D37" si="13">C25</f>
-        <v>2459</v>
-      </c>
-      <c r="D37">
-        <f t="shared" si="13"/>
-        <v>4202</v>
-      </c>
-      <c r="E37" s="2">
-        <f>E25</f>
-        <v>4169</v>
-      </c>
-      <c r="F37" s="2">
-        <f t="shared" ref="F37:G37" si="14">F25</f>
-        <v>2419</v>
-      </c>
-      <c r="G37" s="2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44">
+        <v>8285</v>
+      </c>
+      <c r="C44">
+        <v>13233</v>
+      </c>
+      <c r="D44">
+        <v>15743</v>
+      </c>
+      <c r="E44" s="2">
+        <v>18040</v>
+      </c>
+      <c r="F44" s="2">
+        <v>18029</v>
+      </c>
+      <c r="G44" s="2">
+        <v>19156</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45">
+        <f>C44</f>
+        <v>13233</v>
+      </c>
+      <c r="C45">
+        <f>D44</f>
+        <v>15743</v>
+      </c>
+      <c r="D45">
+        <f>E44</f>
+        <v>18040</v>
+      </c>
+      <c r="E45" s="2">
+        <f>F44</f>
+        <v>18029</v>
+      </c>
+      <c r="F45" s="2">
+        <f>G44</f>
+        <v>19156</v>
+      </c>
+      <c r="G45" s="2">
+        <v>21834</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <f>B45-B44</f>
+        <v>4948</v>
+      </c>
+      <c r="C46">
+        <f t="shared" ref="C46:G46" si="14">C45-C44</f>
+        <v>2510</v>
+      </c>
+      <c r="D46">
         <f t="shared" si="14"/>
-        <v>4246</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>21</v>
-      </c>
-      <c r="B38">
-        <v>5480</v>
-      </c>
-      <c r="C38">
-        <v>4071</v>
-      </c>
-      <c r="D38">
-        <v>5854</v>
-      </c>
-      <c r="E38" s="2">
-        <v>5797</v>
-      </c>
-      <c r="F38" s="2">
-        <v>5813</v>
-      </c>
-      <c r="G38" s="2">
-        <v>4843</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>22</v>
-      </c>
-      <c r="B39" s="2">
-        <v>-823</v>
-      </c>
-      <c r="C39" s="2">
-        <v>-704</v>
-      </c>
-      <c r="D39" s="2">
-        <v>-866</v>
-      </c>
-      <c r="E39" s="2">
-        <v>-908</v>
-      </c>
-      <c r="F39" s="2">
-        <v>-706</v>
-      </c>
-      <c r="G39" s="2">
-        <v>-623</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>23</v>
-      </c>
-      <c r="B40">
-        <v>8285</v>
-      </c>
-      <c r="C40">
-        <v>13233</v>
-      </c>
-      <c r="D40">
-        <v>15743</v>
-      </c>
-      <c r="E40" s="2">
-        <v>18040</v>
-      </c>
-      <c r="F40" s="2">
-        <v>18029</v>
-      </c>
-      <c r="G40" s="2">
-        <v>19156</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>24</v>
-      </c>
-      <c r="B41">
-        <f>C40</f>
-        <v>13233</v>
-      </c>
-      <c r="C41">
-        <f>D40</f>
-        <v>15743</v>
-      </c>
-      <c r="D41">
-        <f>E40</f>
-        <v>18040</v>
-      </c>
-      <c r="E41" s="2">
-        <f>F40</f>
-        <v>18029</v>
-      </c>
-      <c r="F41" s="2">
-        <f>G40</f>
-        <v>19156</v>
-      </c>
-      <c r="G41" s="2">
-        <v>21834</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42">
-        <f>B41-B40</f>
-        <v>4948</v>
-      </c>
-      <c r="C42">
-        <f t="shared" ref="C42:G42" si="15">C41-C40</f>
-        <v>2510</v>
-      </c>
-      <c r="D42">
-        <f t="shared" si="15"/>
         <v>2297</v>
       </c>
-      <c r="E42">
-        <f t="shared" si="15"/>
+      <c r="E46">
+        <f t="shared" si="14"/>
         <v>-11</v>
       </c>
-      <c r="F42">
-        <f t="shared" si="15"/>
+      <c r="F46">
+        <f t="shared" si="14"/>
         <v>1127</v>
       </c>
-      <c r="G42">
-        <f t="shared" si="15"/>
+      <c r="G46">
+        <f t="shared" si="14"/>
         <v>2678</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>25</v>
-      </c>
-      <c r="B43">
-        <f>B38+B39</f>
-        <v>4657</v>
-      </c>
-      <c r="C43">
-        <f t="shared" ref="C43:D43" si="16">C38+C39</f>
-        <v>3367</v>
-      </c>
-      <c r="D43">
-        <f t="shared" si="16"/>
-        <v>4988</v>
-      </c>
-      <c r="E43" s="2">
-        <f>E38+E39</f>
-        <v>4889</v>
-      </c>
-      <c r="F43" s="2">
-        <f t="shared" ref="F43:G43" si="17">F38+F39</f>
-        <v>5107</v>
-      </c>
-      <c r="G43" s="2">
-        <f t="shared" si="17"/>
-        <v>4220</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>26</v>
-      </c>
-      <c r="C44" s="4">
-        <f>C43/B43-1</f>
-        <v>-0.27700236203564521</v>
-      </c>
-      <c r="D44" s="4">
-        <f t="shared" ref="D44:E44" si="18">D43/C43-1</f>
-        <v>0.48143748143748133</v>
-      </c>
-      <c r="E44" s="4">
-        <f t="shared" si="18"/>
-        <v>-1.9847634322373686E-2</v>
-      </c>
-      <c r="F44" s="4">
-        <f>F43/E43-1</f>
-        <v>4.4589895684189029E-2</v>
-      </c>
-      <c r="G44" s="4">
-        <f>G43/F43-1</f>
-        <v>-0.17368317994908944</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>